<commit_message>
Clean up cantril_data_cleaning file
Delete redundant script. Change some file naming.
</commit_message>
<xml_diff>
--- a/Sample1.xlsx
+++ b/Sample1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aramp\cits4407\assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F304AF1-132F-4FFB-91BE-BBF8E91F84BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973A738C-A8F1-4730-B672-51F421263704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{1399D1C8-EE64-724B-BA42-E438291C485C}"/>
+    <workbookView xWindow="71595" yWindow="555" windowWidth="14340" windowHeight="15375" xr2:uid="{1399D1C8-EE64-724B-BA42-E438291C485C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
   <si>
     <t>Year</t>
   </si>
@@ -90,12 +90,6 @@
     <t>BOTTOM PIECES</t>
   </si>
   <si>
-    <t>X's</t>
-  </si>
-  <si>
-    <t>Y's</t>
-  </si>
-  <si>
     <t>sum</t>
   </si>
   <si>
@@ -103,13 +97,31 @@
   </si>
   <si>
     <t>ARE</t>
+  </si>
+  <si>
+    <t>X calc</t>
+  </si>
+  <si>
+    <t>Y calc</t>
+  </si>
+  <si>
+    <t>SQRT X calc</t>
+  </si>
+  <si>
+    <t>SQRT Y calc</t>
+  </si>
+  <si>
+    <t>NPL</t>
+  </si>
+  <si>
+    <t>CORR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -477,23 +489,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5BE2EB-1CB6-8F43-9010-08995C108882}">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="14.31640625" style="1" customWidth="1"/>
-    <col min="2" max="9" width="10.81640625" style="1"/>
-    <col min="10" max="10" width="16.26953125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.2265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.76953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.81640625" style="1"/>
+    <col min="2" max="11" width="10.81640625" style="1"/>
+    <col min="12" max="12" width="16.26953125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13.2265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.76953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,38 +524,38 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A2" s="1">
         <v>2011</v>
       </c>
@@ -562,43 +574,43 @@
       <c r="F2" s="1">
         <v>4.2583500000000001</v>
       </c>
-      <c r="G2" s="1">
+      <c r="I2" s="1">
         <f>SUM(F2*B2)</f>
         <v>8351.0344291050005</v>
       </c>
-      <c r="H2" s="1">
+      <c r="J2" s="1">
         <f>SUM(B2*B2)</f>
         <v>3845898.6978736897</v>
       </c>
-      <c r="I2" s="1">
+      <c r="K2" s="1">
         <f>SUM(F2*F2)</f>
         <v>18.133544722500002</v>
       </c>
-      <c r="K2" s="1">
+      <c r="M2" s="1">
         <v>8</v>
       </c>
-      <c r="L2" s="1">
+      <c r="N2" s="1">
         <f>SUM(B2,B4,B5,B6:B10)</f>
         <v>15892.5929</v>
       </c>
-      <c r="M2" s="1">
+      <c r="O2" s="1">
         <f>SUM(F2,F4:F10)</f>
         <v>25.740749999999998</v>
       </c>
-      <c r="N2" s="1">
-        <f>SUM(G2,G4:G10)</f>
-        <v>51571.882048975</v>
-      </c>
-      <c r="O2" s="1">
-        <f>SUM(H2,H4:H10)</f>
-        <v>31848258.46523679</v>
-      </c>
       <c r="P2" s="1">
         <f>SUM(I2,I4:I10)</f>
+        <v>51571.882048975</v>
+      </c>
+      <c r="Q2" s="1">
+        <f>SUM(J2,J4:J10)</f>
+        <v>31848258.46523679</v>
+      </c>
+      <c r="R2" s="1">
+        <f>SUM(K2,K4:K10)</f>
         <v>85.998758322500009</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A3" s="1">
         <v>2012</v>
       </c>
@@ -614,31 +626,31 @@
       <c r="E3" s="1">
         <v>61.9</v>
       </c>
-      <c r="K3" s="1">
+      <c r="M3" s="1">
         <v>6</v>
       </c>
-      <c r="L3" s="1">
+      <c r="N3" s="1">
         <f>SUM(B14,B17:B21)</f>
         <v>399410.14</v>
       </c>
-      <c r="M3" s="1">
+      <c r="O3" s="1">
         <f>SUM(F14,F17:F21)</f>
         <v>40.378543000000001</v>
       </c>
-      <c r="N3" s="1">
-        <f>SUM(G14,G17:G21)</f>
-        <v>2684793.3117293096</v>
-      </c>
-      <c r="O3" s="1">
-        <f>SUM(H14,H17:H21)</f>
-        <v>26710375398.6436</v>
-      </c>
       <c r="P3" s="1">
         <f>SUM(I14,I17:I21)</f>
+        <v>2684793.3117293096</v>
+      </c>
+      <c r="Q3" s="1">
+        <f>SUM(J14,J17:J21)</f>
+        <v>26710375398.6436</v>
+      </c>
+      <c r="R3" s="1">
+        <f>SUM(K14,K17:K21)</f>
         <v>271.90895077104904</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A4" s="1">
         <v>2015</v>
       </c>
@@ -657,20 +669,20 @@
       <c r="F4" s="1">
         <v>3.36</v>
       </c>
-      <c r="G4" s="1">
-        <f t="shared" ref="G4:G10" si="0">SUM(F4*B4)</f>
+      <c r="I4" s="1">
+        <f>SUM(F4*B4)</f>
         <v>7085.2790399999994</v>
       </c>
-      <c r="H4" s="1">
-        <f t="shared" ref="H4:H10" si="1">SUM(B4*B4)</f>
+      <c r="J4" s="1">
+        <f t="shared" ref="J4:J10" si="0">SUM(B4*B4)</f>
         <v>4446674.7337959995</v>
       </c>
-      <c r="I4" s="1">
-        <f t="shared" ref="I4:I10" si="2">SUM(F4*F4)</f>
+      <c r="K4" s="1">
+        <f t="shared" ref="K4:K9" si="1">SUM(F4*F4)</f>
         <v>11.289599999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A5" s="1">
         <v>2016</v>
       </c>
@@ -689,20 +701,20 @@
       <c r="F5" s="1">
         <v>3.794</v>
       </c>
-      <c r="G5" s="1">
+      <c r="I5" s="1">
+        <f t="shared" ref="I4:I9" si="2">SUM(F5*B5)</f>
+        <v>7972.7950680000004</v>
+      </c>
+      <c r="J5" s="1">
         <f t="shared" si="0"/>
-        <v>7972.7950680000004</v>
-      </c>
-      <c r="H5" s="1">
+        <v>4415974.422084</v>
+      </c>
+      <c r="K5" s="1">
         <f t="shared" si="1"/>
-        <v>4415974.422084</v>
-      </c>
-      <c r="I5" s="1">
-        <f t="shared" si="2"/>
         <v>14.394436000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A6" s="1">
         <v>2017</v>
       </c>
@@ -721,20 +733,20 @@
       <c r="F6" s="1">
         <v>3.6315</v>
       </c>
-      <c r="G6" s="1">
-        <f t="shared" si="0"/>
-        <v>7611.9617294999989</v>
-      </c>
-      <c r="H6" s="1">
-        <f t="shared" si="1"/>
-        <v>4393605.8646489996</v>
-      </c>
       <c r="I6" s="1">
         <f t="shared" si="2"/>
+        <v>7611.9617294999989</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="0"/>
+        <v>4393605.8646489996</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" si="1"/>
         <v>13.187792249999999</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A7" s="1">
         <v>2018</v>
       </c>
@@ -753,20 +765,20 @@
       <c r="F7" s="1">
         <v>3.2033</v>
       </c>
-      <c r="G7" s="1">
-        <f t="shared" si="0"/>
-        <v>6601.0371067000005</v>
-      </c>
-      <c r="H7" s="1">
-        <f t="shared" si="1"/>
-        <v>4246480.3686009999</v>
-      </c>
       <c r="I7" s="1">
         <f t="shared" si="2"/>
+        <v>6601.0371067000005</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="0"/>
+        <v>4246480.3686009999</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="1"/>
         <v>10.26113089</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A8" s="1">
         <v>2019</v>
       </c>
@@ -785,20 +797,20 @@
       <c r="F8" s="1">
         <v>2.5669</v>
       </c>
-      <c r="G8" s="1">
-        <f t="shared" si="0"/>
-        <v>5338.9515251099992</v>
-      </c>
-      <c r="H8" s="1">
-        <f t="shared" si="1"/>
-        <v>4326075.110099609</v>
-      </c>
       <c r="I8" s="1">
         <f t="shared" si="2"/>
+        <v>5338.9515251099992</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="0"/>
+        <v>4326075.110099609</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="1"/>
         <v>6.5889756099999994</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A9" s="1">
         <v>2020</v>
       </c>
@@ -817,30 +829,34 @@
       <c r="F9" s="1">
         <v>2.5228999999999999</v>
       </c>
-      <c r="G9" s="1">
-        <f t="shared" si="0"/>
-        <v>4965.9275088999993</v>
-      </c>
-      <c r="H9" s="1">
-        <f t="shared" si="1"/>
-        <v>3874366.2922809995</v>
-      </c>
       <c r="I9" s="1">
         <f t="shared" si="2"/>
+        <v>4965.9275088999993</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="0"/>
+        <v>3874366.2922809995</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="1"/>
         <v>6.3650244099999993</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L9" s="1" t="s">
+      <c r="M9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="1">
-        <f>SUM(K2*N2)-(L2*M2)</f>
+      <c r="O9" s="1">
+        <f>SUM(M2*P2)-(N2*O2)</f>
         <v>3487.7957011250546</v>
       </c>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="Q9" s="1">
+        <f>SUM(O9/(R13*S13))</f>
+        <v>0.46532028715226437</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A10" s="1">
         <v>2021</v>
       </c>
@@ -859,27 +875,27 @@
       <c r="F10" s="1">
         <v>2.4037999999999999</v>
       </c>
-      <c r="G10" s="1">
+      <c r="I10" s="1">
+        <f>SUM(F10*B10)</f>
+        <v>3644.8956416599995</v>
+      </c>
+      <c r="J10" s="1">
         <f t="shared" si="0"/>
-        <v>3644.8956416599995</v>
-      </c>
-      <c r="H10" s="1">
-        <f t="shared" si="1"/>
         <v>2299182.9758524895</v>
       </c>
-      <c r="I10" s="1">
-        <f t="shared" si="2"/>
+      <c r="K10" s="1">
+        <f>SUM(F10*F10)</f>
         <v>5.7782544399999995</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M10" s="1">
-        <f>SUM(K3*N3)-(L3*M3)</f>
+      <c r="M10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O10" s="1">
+        <f>SUM(M3*P3)-(N3*O3)</f>
         <v>-18839.642250163481</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -888,55 +904,61 @@
         <v>0.46532028715226081</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" ref="C11:F11" si="3">PEARSON(C2:C10, $F$2:$F$10)</f>
+        <f>PEARSON(C2:C10, $F$2:$F$10)</f>
         <v>-0.92159257691056928</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="3"/>
+        <f>PEARSON(D2:D10, $F$2:$F$10)</f>
         <v>-1.7150398199391455E-2</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="3"/>
+        <f>PEARSON(E2:E10, $F$2:$F$10)</f>
         <v>-0.28889099939419094</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="3"/>
+        <f>PEARSON(F2:F10, $F$2:$F$10)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
-      <c r="M12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N12" s="1" t="s">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="O12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="M13" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:17">
-      <c r="K13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L13" s="1" t="s">
+      <c r="N13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M13" s="1">
-        <f>SUM(K2*O2)-(L2*L2)</f>
+      <c r="O13" s="1">
+        <f>SUM(M2*Q2)-(N2*N2)</f>
         <v>2211558.6367639303</v>
       </c>
-      <c r="N13" s="1">
-        <f>SUM(K2*P2)-(M2*M2)</f>
+      <c r="P13" s="1">
+        <f>SUM(M2*R2)-(O2*O2)</f>
         <v>25.403856017500175</v>
       </c>
-      <c r="P13" s="1">
-        <f>SUM(SQRT(M13))</f>
+      <c r="R13" s="1">
+        <f>SUM(SQRT(O13))</f>
         <v>1487.1310086081623</v>
       </c>
-      <c r="Q13" s="1">
-        <f>SUM(SQRT(N13))</f>
+      <c r="S13" s="1">
+        <f>SUM(SQRT(P13))</f>
         <v>5.0402238062907658</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A14" s="1">
         <v>2011</v>
       </c>
@@ -955,49 +977,73 @@
       <c r="F14" s="1">
         <v>6.9772429999999996</v>
       </c>
-      <c r="G14" s="1">
+      <c r="I14" s="1">
         <f>SUM(F14*B14)</f>
         <v>403390.49017630995</v>
       </c>
-      <c r="H14" s="1">
+      <c r="J14" s="1">
         <f>SUM(B14*B14)</f>
         <v>3342593882.1288996</v>
       </c>
-      <c r="I14" s="1">
-        <f t="shared" ref="I14:I16" si="4">SUM(F14*F14)</f>
+      <c r="K14" s="1">
+        <f t="shared" ref="K14" si="3">SUM(F14*F14)</f>
         <v>48.681919881048998</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M14" s="1">
-        <f>SUM(K3*O3)-(L3*L3)</f>
+      <c r="M14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O14" s="1">
+        <f>SUM(M3*Q3)-(N3*N3)</f>
         <v>733792457.04199219</v>
       </c>
-      <c r="N14" s="1">
-        <f>SUM(K3*P3)-(M3*M3)</f>
+      <c r="P14" s="1">
+        <f>SUM(M3*R3)-(O3*O3)</f>
         <v>1.0269698234451425</v>
       </c>
-      <c r="P14" s="1">
-        <f>SUM(SQRT(M14))</f>
+      <c r="R14" s="1">
+        <f>SUM(SQRT(O14))</f>
         <v>27088.603822308603</v>
       </c>
-      <c r="Q14" s="1">
-        <f>SUM(SQRT(N14))</f>
+      <c r="S14" s="1">
+        <f>SUM(SQRT(P14))</f>
         <v>1.0133951960835135</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A15" s="1">
         <v>2012</v>
       </c>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="B15" s="1">
+        <v>59949.245999999999</v>
+      </c>
+      <c r="C15" s="1">
+        <v>8664976</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.79630977000000003</v>
+      </c>
+      <c r="E15" s="1">
+        <v>78.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A16" s="1">
         <v>2013</v>
       </c>
-    </row>
-    <row r="17" spans="1:16">
+      <c r="B16" s="1">
+        <v>62354.824000000001</v>
+      </c>
+      <c r="C16" s="1">
+        <v>8751853</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.65129110000000001</v>
+      </c>
+      <c r="E16" s="1">
+        <v>78.900000000000006</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A17" s="1">
         <v>2014</v>
       </c>
@@ -1016,24 +1062,20 @@
       <c r="F17" s="1">
         <v>6.9009999999999998</v>
       </c>
-      <c r="G17" s="1">
-        <f t="shared" ref="G15:G21" si="5">SUM(F17*B17)</f>
+      <c r="I17" s="1">
+        <f t="shared" ref="I17:I21" si="4">SUM(F17*B17)</f>
         <v>443969.55508999998</v>
       </c>
-      <c r="H17" s="1">
-        <f t="shared" ref="H16:H22" si="6">SUM(B17*B17)</f>
+      <c r="J17" s="1">
+        <f t="shared" ref="J17:J21" si="5">SUM(B17*B17)</f>
         <v>4138875136.1280994</v>
       </c>
-      <c r="I17" s="1">
-        <f t="shared" ref="I17:I23" si="7">SUM(F17*F17)</f>
+      <c r="K17" s="1">
+        <f t="shared" ref="K17:K21" si="6">SUM(F17*F17)</f>
         <v>47.623801</v>
       </c>
-      <c r="M17" s="1">
-        <f>SUM(M9/(P13*Q13))</f>
-        <v>0.46532028715226437</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16">
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A18" s="1">
         <v>2015</v>
       </c>
@@ -1052,24 +1094,24 @@
       <c r="F18" s="1">
         <v>6.5730000000000004</v>
       </c>
-      <c r="G18" s="1">
+      <c r="I18" s="1">
+        <f t="shared" si="4"/>
+        <v>447467.68899000005</v>
+      </c>
+      <c r="J18" s="1">
         <f t="shared" si="5"/>
-        <v>447467.68899000005</v>
-      </c>
-      <c r="H18" s="1">
+        <v>4634427552.1569004</v>
+      </c>
+      <c r="K18" s="1">
         <f t="shared" si="6"/>
-        <v>4634427552.1569004</v>
-      </c>
-      <c r="I18" s="1">
-        <f t="shared" si="7"/>
         <v>43.204329000000008</v>
       </c>
-      <c r="M18" s="1">
-        <f>SUM(M10/(P14*Q14))</f>
+      <c r="O18" s="1">
+        <f>SUM(O10/(R14*S14))</f>
         <v>-0.68628923839145162</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A19" s="1">
         <v>2019</v>
       </c>
@@ -1088,20 +1130,20 @@
       <c r="F19" s="1">
         <v>6.7907999999999999</v>
       </c>
-      <c r="G19" s="1">
+      <c r="I19" s="1">
+        <f t="shared" si="4"/>
+        <v>487458.292128</v>
+      </c>
+      <c r="J19" s="1">
         <f t="shared" si="5"/>
-        <v>487458.292128</v>
-      </c>
-      <c r="H19" s="1">
+        <v>5152678494.2656002</v>
+      </c>
+      <c r="K19" s="1">
         <f t="shared" si="6"/>
-        <v>5152678494.2656002</v>
-      </c>
-      <c r="I19" s="1">
-        <f t="shared" si="7"/>
         <v>46.114964639999997</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A20" s="1">
         <v>2020</v>
       </c>
@@ -1120,20 +1162,20 @@
       <c r="F20" s="1">
         <v>6.5605000000000002</v>
       </c>
-      <c r="G20" s="1">
+      <c r="I20" s="1">
+        <f t="shared" si="4"/>
+        <v>443937.81654499995</v>
+      </c>
+      <c r="J20" s="1">
         <f t="shared" si="5"/>
-        <v>443937.81654499995</v>
-      </c>
-      <c r="H20" s="1">
+        <v>4578997471.5240993</v>
+      </c>
+      <c r="K20" s="1">
         <f t="shared" si="6"/>
-        <v>4578997471.5240993</v>
-      </c>
-      <c r="I20" s="1">
-        <f t="shared" si="7"/>
         <v>43.04016025</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A21" s="1">
         <v>2021</v>
       </c>
@@ -1152,20 +1194,20 @@
       <c r="F21" s="1">
         <v>6.5759999999999996</v>
       </c>
-      <c r="G21" s="1">
+      <c r="I21" s="1">
+        <f t="shared" si="4"/>
+        <v>458569.46879999997</v>
+      </c>
+      <c r="J21" s="1">
         <f t="shared" si="5"/>
-        <v>458569.46879999997</v>
-      </c>
-      <c r="H21" s="1">
+        <v>4862802862.4400005</v>
+      </c>
+      <c r="K21" s="1">
         <f t="shared" si="6"/>
-        <v>4862802862.4400005</v>
-      </c>
-      <c r="I21" s="1">
-        <f t="shared" si="7"/>
         <v>43.243775999999997</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -1174,42 +1216,499 @@
         <v>-0.68628923839136879</v>
       </c>
       <c r="C22" s="1">
-        <f t="shared" ref="C22:F22" si="8">PEARSON(C14:C21, $F$14:$F$21)</f>
+        <f>PEARSON(C14:C21, $F$14:$F$21)</f>
         <v>-0.74858841330989667</v>
       </c>
       <c r="D22" s="1">
+        <f t="shared" ref="D22:F22" si="7">PEARSON(D14:D21, $F$14:$F$21)</f>
+        <v>0.13869947387847217</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="7"/>
+        <v>-0.12705848169847878</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="I24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A25" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2763.8289</v>
+      </c>
+      <c r="C25" s="1">
+        <v>27266398</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2.4902443999999999</v>
+      </c>
+      <c r="E25" s="1">
+        <v>67.3</v>
+      </c>
+      <c r="F25" s="1">
+        <v>4.474119</v>
+      </c>
+      <c r="H25" s="1">
+        <v>4.474119</v>
+      </c>
+      <c r="I25" s="1">
+        <f>SUM(F25*B25)</f>
+        <v>12365.6993942391</v>
+      </c>
+      <c r="J25" s="1">
+        <f>SUM(B25*B25)</f>
+        <v>7638750.1884752102</v>
+      </c>
+      <c r="K25" s="1">
+        <f>SUM(F25*F25)</f>
+        <v>20.017740826160999</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A26" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B26" s="1">
+        <v>3152.2932000000001</v>
+      </c>
+      <c r="C26" s="1">
+        <v>27462110</v>
+      </c>
+      <c r="D26" s="1">
+        <v>2.0318909000000001</v>
+      </c>
+      <c r="E26" s="1">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="F26" s="1">
+        <v>4.5140000000000002</v>
+      </c>
+      <c r="H26" s="1">
+        <v>4.5140000000000002</v>
+      </c>
+      <c r="I26" s="1">
+        <f>SUM(F26*B26)</f>
+        <v>14229.451504800001</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" ref="J26:J31" si="8">SUM(B26*B26)</f>
+        <v>9936952.4187662397</v>
+      </c>
+      <c r="K26" s="1">
+        <f t="shared" ref="K26:K31" si="9">SUM(F26*F26)</f>
+        <v>20.376196000000004</v>
+      </c>
+      <c r="M26" s="1">
+        <v>7</v>
+      </c>
+      <c r="N26" s="1">
+        <f>SUM(B25:B31)</f>
+        <v>23557.749400000001</v>
+      </c>
+      <c r="O26" s="1">
+        <f>SUM(F25:F31)</f>
+        <v>33.673419000000003</v>
+      </c>
+      <c r="P26" s="1">
+        <f>SUM(I25:I31)</f>
+        <v>113800.5112608491</v>
+      </c>
+      <c r="Q26" s="1">
+        <f>SUM(J25:J31)</f>
+        <v>80166136.691988468</v>
+      </c>
+      <c r="R26" s="1">
+        <f>SUM(K25:K31)</f>
+        <v>162.33197911616099</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A27" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B27" s="1">
+        <v>3260.0349999999999</v>
+      </c>
+      <c r="C27" s="1">
+        <v>27610328</v>
+      </c>
+      <c r="D27" s="1">
+        <v>2.0209830000000002</v>
+      </c>
+      <c r="E27" s="1">
+        <v>67.5</v>
+      </c>
+      <c r="F27" s="1">
+        <v>4.7930000000000001</v>
+      </c>
+      <c r="H27" s="1">
+        <v>4.7930000000000001</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" ref="I27:I31" si="10">SUM(F27*B27)</f>
+        <v>15625.347755000001</v>
+      </c>
+      <c r="J27" s="1">
         <f t="shared" si="8"/>
-        <v>0.13869947387847217</v>
-      </c>
-      <c r="E22" s="1">
+        <v>10627828.201225</v>
+      </c>
+      <c r="K27" s="1">
+        <f t="shared" si="9"/>
+        <v>22.972849</v>
+      </c>
+      <c r="M27" s="1">
+        <v>6</v>
+      </c>
+      <c r="N27" s="1">
+        <f>SUM(B38,B41:B45)</f>
+        <v>1515.1242</v>
+      </c>
+      <c r="O27" s="1">
+        <f>SUM(F38,F41:F45)</f>
+        <v>0</v>
+      </c>
+      <c r="P27" s="1">
+        <f>SUM(I30,I33:I37)</f>
+        <v>18271.84392033</v>
+      </c>
+      <c r="Q27" s="1">
+        <f>SUM(J30,J33:J37)</f>
+        <v>13833251.255002409</v>
+      </c>
+      <c r="R27" s="1">
+        <f>SUM(K30,K33:K37)</f>
+        <v>24.134621290000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A28" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B28" s="1">
+        <v>3244.6743000000001</v>
+      </c>
+      <c r="C28" s="1">
+        <v>27861186</v>
+      </c>
+      <c r="D28" s="1">
+        <v>2.1463551999999999</v>
+      </c>
+      <c r="E28" s="1">
+        <v>68.8</v>
+      </c>
+      <c r="F28" s="1">
+        <v>4.9619999999999997</v>
+      </c>
+      <c r="H28" s="1">
+        <v>4.9619999999999997</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" si="10"/>
+        <v>16100.073876599999</v>
+      </c>
+      <c r="J28" s="1">
         <f t="shared" si="8"/>
-        <v>-0.12705848169847878</v>
-      </c>
-      <c r="F22" s="1">
+        <v>10527911.313080491</v>
+      </c>
+      <c r="K28" s="1">
+        <f t="shared" si="9"/>
+        <v>24.621443999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A29" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B29" s="1">
+        <v>3495.5288</v>
+      </c>
+      <c r="C29" s="1">
+        <v>28183424</v>
+      </c>
+      <c r="D29" s="1">
+        <v>2.1892299999999998</v>
+      </c>
+      <c r="E29" s="1">
+        <v>68.900000000000006</v>
+      </c>
+      <c r="F29" s="1">
+        <v>4.8803999999999998</v>
+      </c>
+      <c r="H29" s="1">
+        <v>4.8803999999999998</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" si="10"/>
+        <v>17059.57875552</v>
+      </c>
+      <c r="J29" s="1">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16">
-      <c r="L28" s="1">
-        <f>(1920-1600)</f>
-        <v>320</v>
-      </c>
-      <c r="M28" s="1">
-        <f>SUM(5880-4900)</f>
-        <v>980</v>
-      </c>
-      <c r="N28" s="1">
-        <f>SUM(SQRT(L28))</f>
-        <v>17.888543819998318</v>
-      </c>
-      <c r="O28" s="1">
-        <f>SUM(SQRT(M28))</f>
-        <v>31.304951684997057</v>
-      </c>
-      <c r="P28" s="1">
-        <f>O28*N28</f>
-        <v>560</v>
+        <v>12218721.59162944</v>
+      </c>
+      <c r="K29" s="1">
+        <f t="shared" si="9"/>
+        <v>23.81830416</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A30" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B30" s="1">
+        <v>3719.3078999999998</v>
+      </c>
+      <c r="C30" s="1">
+        <v>28506718</v>
+      </c>
+      <c r="D30" s="1">
+        <v>2.2100057999999998</v>
+      </c>
+      <c r="E30" s="1">
+        <v>69</v>
+      </c>
+      <c r="F30" s="1">
+        <v>4.9127000000000001</v>
+      </c>
+      <c r="H30" s="1">
+        <v>4.9127000000000001</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" si="10"/>
+        <v>18271.84392033</v>
+      </c>
+      <c r="J30" s="1">
+        <f t="shared" si="8"/>
+        <v>13833251.255002409</v>
+      </c>
+      <c r="K30" s="1">
+        <f t="shared" si="9"/>
+        <v>24.134621290000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A31" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B31" s="1">
+        <v>3922.0812999999998</v>
+      </c>
+      <c r="C31" s="1">
+        <v>28832500</v>
+      </c>
+      <c r="D31" s="1">
+        <v>2.2856154000000002</v>
+      </c>
+      <c r="E31" s="1">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="F31" s="1">
+        <v>5.1372</v>
+      </c>
+      <c r="H31" s="1">
+        <v>5.1372</v>
+      </c>
+      <c r="I31" s="1">
+        <f t="shared" si="10"/>
+        <v>20148.51605436</v>
+      </c>
+      <c r="J31" s="1">
+        <f t="shared" si="8"/>
+        <v>15382721.723809689</v>
+      </c>
+      <c r="K31" s="1">
+        <f t="shared" si="9"/>
+        <v>26.390823839999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="M33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O33" s="1">
+        <f>SUM(M26*P26)-(N26*O26)</f>
+        <v>3333.6125827450305</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q33" s="1">
+        <f>SUM(O33/(R37*S37))</f>
+        <v>0.86010376000089017</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A34">
+        <v>2020</v>
+      </c>
+      <c r="B34">
+        <v>711.35530000000006</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O34" s="1">
+        <f>SUM(M27*P27)-(N27*O27)</f>
+        <v>109631.06352198</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A35">
+        <v>2019</v>
+      </c>
+      <c r="B35">
+        <v>729.65845000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A36">
+        <v>2018</v>
+      </c>
+      <c r="B36">
+        <v>740.44824000000006</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R36" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S36" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A37">
+        <v>2011</v>
+      </c>
+      <c r="B37">
+        <v>807.66499999999996</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O37" s="1">
+        <f>SUM(M26*Q26)-(N26*N26)</f>
+        <v>6195400.0507189035</v>
+      </c>
+      <c r="P37" s="1">
+        <f>SUM(M26*R26)-(O26*O26)</f>
+        <v>2.4247066635657575</v>
+      </c>
+      <c r="R37" s="1">
+        <f>SUM(SQRT(O37))</f>
+        <v>2489.0560561624366</v>
+      </c>
+      <c r="S37" s="1">
+        <f>SUM(SQRT(P37))</f>
+        <v>1.5571469627385071</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A38">
+        <v>2016</v>
+      </c>
+      <c r="B38">
+        <v>764.33659999999998</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O38" s="1">
+        <f>SUM(M27*Q27)-(N27*N27)</f>
+        <v>80703906.188588813</v>
+      </c>
+      <c r="P38" s="1">
+        <f>SUM(M27*R27)-(O27*O27)</f>
+        <v>144.80772774000002</v>
+      </c>
+      <c r="R38" s="1">
+        <f>SUM(SQRT(O38))</f>
+        <v>8983.5352834276109</v>
+      </c>
+      <c r="S38" s="1">
+        <f>SUM(SQRT(P38))</f>
+        <v>12.03360825937092</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A39">
+        <v>2015</v>
+      </c>
+      <c r="B39">
+        <v>781.57929999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A40">
+        <v>2014</v>
+      </c>
+      <c r="B40">
+        <v>831.29485999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A41">
+        <v>2017</v>
+      </c>
+      <c r="B41">
+        <v>750.7876</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O41" s="1">
+        <f>SUM(O33/(R37*S37))</f>
+        <v>0.86010376000089017</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="O42" s="1">
+        <f>SUM(O34/(R38*S38))</f>
+        <v>1.0141226436889357</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Standard deviation calculation working for gpd and population
Create awk script to generate sd for all files and calculate mean
</commit_message>
<xml_diff>
--- a/Sample1.xlsx
+++ b/Sample1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aramp\cits4407\assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973A738C-A8F1-4730-B672-51F421263704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9A3835-AD42-4A06-8FAD-F26B2810DA30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="71595" yWindow="555" windowWidth="14340" windowHeight="15375" xr2:uid="{1399D1C8-EE64-724B-BA42-E438291C485C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{1399D1C8-EE64-724B-BA42-E438291C485C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="30">
   <si>
     <t>Year</t>
   </si>
@@ -115,13 +115,22 @@
   </si>
   <si>
     <t>CORR</t>
+  </si>
+  <si>
+    <t>EXCEL PEARSON - NPL</t>
+  </si>
+  <si>
+    <t>BWI</t>
+  </si>
+  <si>
+    <t>EXCEL PEARSON - JPN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -489,13 +498,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5BE2EB-1CB6-8F43-9010-08995C108882}">
-  <dimension ref="A1:S42"/>
+  <dimension ref="A1:W58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.31640625" style="1" customWidth="1"/>
     <col min="2" max="11" width="10.81640625" style="1"/>
@@ -505,7 +514,7 @@
     <col min="15" max="16384" width="10.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,8 +563,11 @@
       <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="V1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
       <c r="A2" s="1">
         <v>2011</v>
       </c>
@@ -609,8 +621,17 @@
         <f>SUM(K2,K4:K10)</f>
         <v>85.998758322500009</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="U2">
+        <v>2011</v>
+      </c>
+      <c r="V2">
+        <v>2763.8289</v>
+      </c>
+      <c r="W2">
+        <v>4.474119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
       <c r="A3" s="1">
         <v>2012</v>
       </c>
@@ -649,8 +670,17 @@
         <f>SUM(K14,K17:K21)</f>
         <v>271.90895077104904</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="U3">
+        <v>2014</v>
+      </c>
+      <c r="V3">
+        <v>3152.2932000000001</v>
+      </c>
+      <c r="W3">
+        <v>4.5140000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
       <c r="A4" s="1">
         <v>2015</v>
       </c>
@@ -681,8 +711,17 @@
         <f t="shared" ref="K4:K9" si="1">SUM(F4*F4)</f>
         <v>11.289599999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="U4">
+        <v>2015</v>
+      </c>
+      <c r="V4">
+        <v>3260.0349999999999</v>
+      </c>
+      <c r="W4">
+        <v>4.7930000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
       <c r="A5" s="1">
         <v>2016</v>
       </c>
@@ -702,7 +741,7 @@
         <v>3.794</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" ref="I4:I9" si="2">SUM(F5*B5)</f>
+        <f t="shared" ref="I5:I9" si="2">SUM(F5*B5)</f>
         <v>7972.7950680000004</v>
       </c>
       <c r="J5" s="1">
@@ -713,8 +752,17 @@
         <f t="shared" si="1"/>
         <v>14.394436000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="U5">
+        <v>2016</v>
+      </c>
+      <c r="V5">
+        <v>3244.6743000000001</v>
+      </c>
+      <c r="W5">
+        <v>4.9619999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6" s="1">
         <v>2017</v>
       </c>
@@ -745,8 +793,17 @@
         <f t="shared" si="1"/>
         <v>13.187792249999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="U6">
+        <v>2017</v>
+      </c>
+      <c r="V6">
+        <v>3495.5288</v>
+      </c>
+      <c r="W6">
+        <v>4.8803999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7" s="1">
         <v>2018</v>
       </c>
@@ -777,8 +834,17 @@
         <f t="shared" si="1"/>
         <v>10.26113089</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="U7">
+        <v>2018</v>
+      </c>
+      <c r="V7">
+        <v>3719.3078999999998</v>
+      </c>
+      <c r="W7">
+        <v>4.9127000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8" s="1">
         <v>2019</v>
       </c>
@@ -809,8 +875,17 @@
         <f t="shared" si="1"/>
         <v>6.5889756099999994</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="U8">
+        <v>2019</v>
+      </c>
+      <c r="V8">
+        <v>3922.0812999999998</v>
+      </c>
+      <c r="W8">
+        <v>5.1372</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
       <c r="A9" s="1">
         <v>2020</v>
       </c>
@@ -855,8 +930,12 @@
         <f>SUM(O9/(R13*S13))</f>
         <v>0.46532028715226437</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="V9" s="1">
+        <f>PEARSON(V2:V8, $W$2:$W$8)</f>
+        <v>0.86010376000085842</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
       <c r="A10" s="1">
         <v>2021</v>
       </c>
@@ -895,7 +974,7 @@
         <v>-18839.642250163481</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:23">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -919,8 +998,11 @@
         <f>PEARSON(F2:F10, $F$2:$F$10)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="V11" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
       <c r="O12" s="1" t="s">
         <v>21</v>
       </c>
@@ -933,8 +1015,17 @@
       <c r="S12" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="U12">
+        <v>2020</v>
+      </c>
+      <c r="V12">
+        <v>13545.674000000001</v>
+      </c>
+      <c r="W12">
+        <v>3.4664999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
       <c r="M13" s="1" t="s">
         <v>19</v>
       </c>
@@ -957,8 +1048,17 @@
         <f>SUM(SQRT(P13))</f>
         <v>5.0402238062907658</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="U13">
+        <v>2021</v>
+      </c>
+      <c r="V13">
+        <v>14840.913</v>
+      </c>
+      <c r="W13">
+        <v>3.4710999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
       <c r="A14" s="1">
         <v>2011</v>
       </c>
@@ -1008,8 +1108,12 @@
         <f>SUM(SQRT(P14))</f>
         <v>1.0133951960835135</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="V14" s="1">
+        <f>PEARSON(V12:V13, $W$12:$W$13)</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
       <c r="A15" s="1">
         <v>2012</v>
       </c>
@@ -1026,7 +1130,7 @@
         <v>78.7</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:23">
       <c r="A16" s="1">
         <v>2013</v>
       </c>
@@ -1043,7 +1147,7 @@
         <v>78.900000000000006</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:23">
       <c r="A17" s="1">
         <v>2014</v>
       </c>
@@ -1074,8 +1178,11 @@
         <f t="shared" ref="K17:K21" si="6">SUM(F17*F17)</f>
         <v>47.623801</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="V17" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23">
       <c r="A18" s="1">
         <v>2015</v>
       </c>
@@ -1110,8 +1217,17 @@
         <f>SUM(O10/(R14*S14))</f>
         <v>-0.68628923839145162</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="U18" s="1">
+        <v>2011</v>
+      </c>
+      <c r="V18">
+        <v>38149.616999999998</v>
+      </c>
+      <c r="W18">
+        <v>6.0590979999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23">
       <c r="A19" s="1">
         <v>2019</v>
       </c>
@@ -1142,8 +1258,17 @@
         <f t="shared" si="6"/>
         <v>46.114964639999997</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="U19" s="1">
+        <v>2014</v>
+      </c>
+      <c r="V19">
+        <v>39739.542999999998</v>
+      </c>
+      <c r="W19">
+        <v>5.9870000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23">
       <c r="A20" s="1">
         <v>2020</v>
       </c>
@@ -1174,8 +1299,17 @@
         <f t="shared" si="6"/>
         <v>43.04016025</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="U20" s="1">
+        <v>2015</v>
+      </c>
+      <c r="V20">
+        <v>40402.582000000002</v>
+      </c>
+      <c r="W20">
+        <v>5.9210000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23">
       <c r="A21" s="1">
         <v>2021</v>
       </c>
@@ -1206,8 +1340,17 @@
         <f t="shared" si="6"/>
         <v>43.243775999999997</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="U21" s="1">
+        <v>2016</v>
+      </c>
+      <c r="V21">
+        <v>40727.97</v>
+      </c>
+      <c r="W21">
+        <v>5.92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -1231,8 +1374,28 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="U22" s="1">
+        <v>2017</v>
+      </c>
+      <c r="V22">
+        <v>41444.214999999997</v>
+      </c>
+      <c r="W22">
+        <v>5.915</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23">
+      <c r="U23" s="1">
+        <v>2018</v>
+      </c>
+      <c r="V23">
+        <v>41739.203000000001</v>
+      </c>
+      <c r="W23">
+        <v>5.8860999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23">
       <c r="I24" s="1" t="s">
         <v>13</v>
       </c>
@@ -1242,8 +1405,17 @@
       <c r="K24" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="U24" s="1">
+        <v>2019</v>
+      </c>
+      <c r="V24">
+        <v>41697.410000000003</v>
+      </c>
+      <c r="W24">
+        <v>5.8708</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23">
       <c r="A25" s="1">
         <v>2011</v>
       </c>
@@ -1298,8 +1470,17 @@
       <c r="S25" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="U25" s="1">
+        <v>2020</v>
+      </c>
+      <c r="V25" s="1">
+        <v>39935.464999999997</v>
+      </c>
+      <c r="W25">
+        <v>5.9405000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23">
       <c r="A26" s="1">
         <v>2014</v>
       </c>
@@ -1356,8 +1537,17 @@
         <f>SUM(K25:K31)</f>
         <v>162.33197911616099</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="U26" s="1">
+        <v>2021</v>
+      </c>
+      <c r="V26" s="1">
+        <v>40784.383000000002</v>
+      </c>
+      <c r="W26">
+        <v>6.0388999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23">
       <c r="A27" s="1">
         <v>2015</v>
       </c>
@@ -1395,12 +1585,12 @@
         <v>6</v>
       </c>
       <c r="N27" s="1">
-        <f>SUM(B38,B41:B45)</f>
-        <v>1515.1242</v>
+        <f>SUM(V6,B41:B44)</f>
+        <v>3495.5288</v>
       </c>
       <c r="O27" s="1">
-        <f>SUM(F38,F41:F45)</f>
-        <v>0</v>
+        <f>SUM(W6,F41:F44)</f>
+        <v>4.8803999999999998</v>
       </c>
       <c r="P27" s="1">
         <f>SUM(I30,I33:I37)</f>
@@ -1414,8 +1604,12 @@
         <f>SUM(K30,K33:K37)</f>
         <v>24.134621290000002</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="V27" s="1">
+        <f>PEARSON(V18:V26, $W$18:$W$26)</f>
+        <v>-0.77436831688680807</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23">
       <c r="A28" s="1">
         <v>2016</v>
       </c>
@@ -1450,7 +1644,7 @@
         <v>24.621443999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:23">
       <c r="A29" s="1">
         <v>2017</v>
       </c>
@@ -1485,7 +1679,7 @@
         <v>23.81830416</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:23">
       <c r="A30" s="1">
         <v>2018</v>
       </c>
@@ -1520,7 +1714,7 @@
         <v>24.134621290000002</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:23">
       <c r="A31" s="1">
         <v>2019</v>
       </c>
@@ -1555,7 +1749,7 @@
         <v>26.390823839999999</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:19">
       <c r="M33" s="1" t="s">
         <v>19</v>
       </c>
@@ -1574,36 +1768,16 @@
         <v>0.86010376000089017</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A34">
-        <v>2020</v>
-      </c>
-      <c r="B34">
-        <v>711.35530000000006</v>
-      </c>
+    <row r="34" spans="1:19">
       <c r="M34" s="1" t="s">
         <v>20</v>
       </c>
       <c r="O34" s="1">
         <f>SUM(M27*P27)-(N27*O27)</f>
-        <v>109631.06352198</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A35">
-        <v>2019</v>
-      </c>
-      <c r="B35">
-        <v>729.65845000000002</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A36">
-        <v>2018</v>
-      </c>
-      <c r="B36">
-        <v>740.44824000000006</v>
-      </c>
+        <v>92571.484766459995</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19">
       <c r="O36" s="1" t="s">
         <v>21</v>
       </c>
@@ -1617,13 +1791,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A37">
-        <v>2011</v>
-      </c>
-      <c r="B37">
-        <v>807.66499999999996</v>
-      </c>
+    <row r="37" spans="1:19">
       <c r="M37" s="1" t="s">
         <v>19</v>
       </c>
@@ -1647,56 +1815,28 @@
         <v>1.5571469627385071</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A38">
-        <v>2016</v>
-      </c>
-      <c r="B38">
-        <v>764.33659999999998</v>
-      </c>
+    <row r="38" spans="1:19">
       <c r="M38" s="1" t="s">
         <v>20</v>
       </c>
       <c r="O38" s="1">
         <f>SUM(M27*Q27)-(N27*N27)</f>
-        <v>80703906.188588813</v>
+        <v>70780785.93838501</v>
       </c>
       <c r="P38" s="1">
         <f>SUM(M27*R27)-(O27*O27)</f>
-        <v>144.80772774000002</v>
+        <v>120.98942358000002</v>
       </c>
       <c r="R38" s="1">
         <f>SUM(SQRT(O38))</f>
-        <v>8983.5352834276109</v>
+        <v>8413.1317556772519</v>
       </c>
       <c r="S38" s="1">
         <f>SUM(SQRT(P38))</f>
-        <v>12.03360825937092</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A39">
-        <v>2015</v>
-      </c>
-      <c r="B39">
-        <v>781.57929999999999</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A40">
-        <v>2014</v>
-      </c>
-      <c r="B40">
-        <v>831.29485999999997</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A41">
-        <v>2017</v>
-      </c>
-      <c r="B41">
-        <v>750.7876</v>
-      </c>
+        <v>10.999519243130583</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19">
       <c r="M41" s="1" t="s">
         <v>25</v>
       </c>
@@ -1705,10 +1845,256 @@
         <v>0.86010376000089017</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:19">
       <c r="O42" s="1">
         <f>SUM(O34/(R38*S38))</f>
-        <v>1.0141226436889357</v>
+        <v>1.0003358546465779</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19">
+      <c r="I44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19">
+      <c r="A45">
+        <v>2020</v>
+      </c>
+      <c r="B45">
+        <v>13545.674000000001</v>
+      </c>
+      <c r="C45">
+        <v>2546404</v>
+      </c>
+      <c r="D45">
+        <v>8.6789120000000004</v>
+      </c>
+      <c r="E45">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="F45">
+        <v>3.4664999999999999</v>
+      </c>
+      <c r="I45" s="1">
+        <f>SUM(F45*B45)</f>
+        <v>46956.078921</v>
+      </c>
+      <c r="J45" s="1">
+        <f>SUM(B45*B45)</f>
+        <v>183485284.11427602</v>
+      </c>
+      <c r="K45" s="1">
+        <f>SUM(F45*F45)</f>
+        <v>12.016622249999999</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S45" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19">
+      <c r="A46">
+        <v>2021</v>
+      </c>
+      <c r="B46">
+        <v>14840.913</v>
+      </c>
+      <c r="C46">
+        <v>2588424</v>
+      </c>
+      <c r="D46">
+        <v>10.546963</v>
+      </c>
+      <c r="E46">
+        <v>61.1</v>
+      </c>
+      <c r="F46">
+        <v>3.4710999999999999</v>
+      </c>
+      <c r="I46" s="1">
+        <f>SUM(F46*B46)</f>
+        <v>51514.293114300002</v>
+      </c>
+      <c r="J46" s="1">
+        <f>SUM(B46*B46)</f>
+        <v>220252698.67356902</v>
+      </c>
+      <c r="K46" s="1">
+        <f t="shared" ref="K46:K51" si="11">SUM(F46*F46)</f>
+        <v>12.048535209999999</v>
+      </c>
+      <c r="M46" s="1">
+        <v>2</v>
+      </c>
+      <c r="N46" s="1">
+        <f>SUM(B45:B46)</f>
+        <v>28386.587</v>
+      </c>
+      <c r="O46" s="1">
+        <f>SUM(F45:F46)</f>
+        <v>6.9375999999999998</v>
+      </c>
+      <c r="P46" s="1">
+        <f>SUM(I45:I46)</f>
+        <v>98470.37203530001</v>
+      </c>
+      <c r="Q46" s="1">
+        <f>SUM(J45:J46)</f>
+        <v>403737982.78784502</v>
+      </c>
+      <c r="R46" s="1">
+        <f>SUM(K45:K46)</f>
+        <v>24.065157459999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19">
+      <c r="M47" s="1">
+        <v>6</v>
+      </c>
+      <c r="N47" s="1">
+        <f>SUM(V26,B61:B64)</f>
+        <v>40784.383000000002</v>
+      </c>
+      <c r="O47" s="1">
+        <f>SUM(W26,F61:F65)</f>
+        <v>6.0388999999999999</v>
+      </c>
+      <c r="P47" s="1">
+        <f>SUM(I50,I53:I57)</f>
+        <v>0</v>
+      </c>
+      <c r="Q47" s="1">
+        <f>SUM(J50,J53:J57)</f>
+        <v>0</v>
+      </c>
+      <c r="R47" s="1">
+        <f>SUM(K50,K53:K57)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="13:19">
+      <c r="M49" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O49" s="1">
+        <f>SUM(M46*P46)-(N46*O46)</f>
+        <v>5.9580994000425562</v>
+      </c>
+      <c r="P49" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q49" s="1">
+        <f>SUM(O49/(R53*S53))</f>
+        <v>0.9999999999397633</v>
+      </c>
+    </row>
+    <row r="50" spans="13:19">
+      <c r="M50" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O50" s="1">
+        <f>SUM(M47*P47)-(N47*O47)</f>
+        <v>-246292.81049870001</v>
+      </c>
+    </row>
+    <row r="52" spans="13:19">
+      <c r="O52" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P52" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R52" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S52" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="13:19">
+      <c r="M53" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O53" s="1">
+        <f>SUM(M46*Q46)-(N46*N46)</f>
+        <v>1677644.0671210289</v>
+      </c>
+      <c r="P53" s="1">
+        <f>SUM(M46*R46)-(O46*O46)</f>
+        <v>2.116000000285112E-5</v>
+      </c>
+      <c r="R53" s="1">
+        <f>SUM(SQRT(O53))</f>
+        <v>1295.2390000000112</v>
+      </c>
+      <c r="S53" s="1">
+        <f>SUM(SQRT(P53))</f>
+        <v>4.6000000003099048E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="13:19">
+      <c r="M54" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O54" s="1">
+        <f>SUM(M47*Q47)-(N47*N47)</f>
+        <v>-1663365896.6906891</v>
+      </c>
+      <c r="P54" s="1">
+        <f>SUM(M47*R47)-(O47*O47)</f>
+        <v>-36.468313209999998</v>
+      </c>
+      <c r="R54" s="1" t="e">
+        <f>SUM(SQRT(O54))</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="S54" s="1" t="e">
+        <f>SUM(SQRT(P54))</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="57" spans="13:19">
+      <c r="M57" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O57" s="1">
+        <f>SUM(O49/(R53*S53))</f>
+        <v>0.9999999999397633</v>
+      </c>
+    </row>
+    <row r="58" spans="13:19">
+      <c r="O58" s="1" t="e">
+        <f>SUM(O50/(R54*S54))</f>
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Can't get the abs comparison to work
</commit_message>
<xml_diff>
--- a/Sample1.xlsx
+++ b/Sample1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aramp\cits4407\assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9A3835-AD42-4A06-8FAD-F26B2810DA30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C849E8-5D1D-498B-8B39-FEC7CFAA4528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{1399D1C8-EE64-724B-BA42-E438291C485C}"/>
+    <workbookView xWindow="1800" yWindow="444" windowWidth="14940" windowHeight="12870" xr2:uid="{1399D1C8-EE64-724B-BA42-E438291C485C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -500,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5BE2EB-1CB6-8F43-9010-08995C108882}">
   <dimension ref="A1:W58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15"/>
@@ -1777,6 +1777,24 @@
         <v>92571.484766459995</v>
       </c>
     </row>
+    <row r="35" spans="1:19">
+      <c r="B35" s="1">
+        <f>SUM(B11+B22)/2</f>
+        <v>-0.11048447561955399</v>
+      </c>
+      <c r="C35" s="1">
+        <f t="shared" ref="C35:E35" si="11">SUM(C11+C22)/2</f>
+        <v>-0.83509049511023292</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="11"/>
+        <v>6.0774537839540357E-2</v>
+      </c>
+      <c r="E35" s="1">
+        <f t="shared" si="11"/>
+        <v>-0.20797474054633486</v>
+      </c>
+    </row>
     <row r="36" spans="1:19">
       <c r="O36" s="1" t="s">
         <v>21</v>
@@ -1943,7 +1961,7 @@
         <v>220252698.67356902</v>
       </c>
       <c r="K46" s="1">
-        <f t="shared" ref="K46:K51" si="11">SUM(F46*F46)</f>
+        <f t="shared" ref="K46" si="12">SUM(F46*F46)</f>
         <v>12.048535209999999</v>
       </c>
       <c r="M46" s="1">

</xml_diff>